<commit_message>
add image to templates
</commit_message>
<xml_diff>
--- a/public/templates/quotation-template-ezy.xlsx
+++ b/public/templates/quotation-template-ezy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThanapongChun\Desktop\Work\ezyaccount_nextjs\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MYWORK\ezyaccount_nextjs\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F7A1B8-A3AD-4F7B-8CBC-5E41E2061C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F08083-2684-4893-BC73-BCB05A7909B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUOTE" sheetId="13" r:id="rId1"/>
@@ -139,8 +139,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -288,7 +288,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -300,21 +300,21 @@
     </font>
     <font>
       <sz val="16"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -326,7 +326,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -334,7 +334,7 @@
       <b/>
       <sz val="28"/>
       <color theme="4"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -349,7 +349,7 @@
       <u/>
       <sz val="10"/>
       <color indexed="12"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -362,14 +362,14 @@
     <font>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -377,7 +377,7 @@
       <b/>
       <sz val="9"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -385,7 +385,7 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Cordia New"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -826,7 +826,7 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -845,7 +845,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -958,19 +958,19 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -980,22 +980,22 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1027,95 +1027,95 @@
     <xf numFmtId="0" fontId="37" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="37" fillId="20" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="37" fillId="20" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="45">
-    <cellStyle name="20% - ส่วนที่ถูกเน้น1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - ส่วนที่ถูกเน้น6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - ส่วนที่ถูกเน้น6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - ส่วนที่ถูกเน้น6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="28" builtinId="3"/>
+    <cellStyle name="Currency" xfId="44" builtinId="4"/>
+    <cellStyle name="Explanatory Text" xfId="29" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="30" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="31" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="32" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="34" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="การคำนวณ" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="ข้อความเตือน" xfId="43" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="ข้อความอธิบาย" xfId="29" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="จุลภาค" xfId="28" builtinId="3"/>
-    <cellStyle name="ชื่อเรื่อง" xfId="41" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="เซลล์ตรวจสอบ" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="เซลล์ที่มีลิงก์" xfId="37" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="ดี" xfId="30" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="ปกติ" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="ป้อนค่า" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="ปานกลาง" xfId="38" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="ผลรวม" xfId="42" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="แย่" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="สกุลเงิน" xfId="44" builtinId="4"/>
-    <cellStyle name="ส่วนที่ถูกเน้น1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="ส่วนที่ถูกเน้น6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="แสดงผล" xfId="40" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="หมายเหตุ" xfId="39" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 1" xfId="31" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 2" xfId="32" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 3" xfId="33" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="หัวเรื่อง 4" xfId="34" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="41" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1205,23 +1205,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1392621</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>663465</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>45983</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="รูปภาพ 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{787AE31D-A5B9-6CDB-444F-2EB28E640F0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9958C8AE-3AA3-65D6-9BC8-21083B81D206}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1230,7 +1230,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1243,82 +1243,14 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4159250" y="0"/>
-          <a:ext cx="2492375" cy="2492375"/>
+          <a:off x="3304190" y="0"/>
+          <a:ext cx="3350172" cy="2850931"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>666747</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Right Triangle 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E039512-90BE-070A-3DF6-B4EAECAEAADC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="3409950" y="0"/>
-          <a:ext cx="3248022" cy="2543175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rtTriangle">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="C6D9F1">
-            <a:alpha val="40000"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="th-TH" sz="1100" kern="1200"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1884,8 +1816,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" topLeftCell="A4" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1901,13 +1833,13 @@
     <col min="10" max="10" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="39.75" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>27</v>
       </c>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
@@ -1916,7 +1848,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +1861,7 @@
       <c r="H3" s="10"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1939,7 +1871,7 @@
       <c r="E4" s="9"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1956,7 +1888,7 @@
       </c>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1966,7 +1898,7 @@
       <c r="E6" s="9"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -2002,7 +1934,7 @@
       <c r="H10" s="16"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
@@ -2013,7 +1945,7 @@
       <c r="H11" s="16"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
@@ -2021,7 +1953,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -2042,12 +1974,12 @@
       <c r="G14" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="56" t="s">
+      <c r="H14" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="57"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I14" s="56"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>4</v>
       </c>
@@ -2061,11 +1993,11 @@
       <c r="G15" s="39">
         <v>200</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="57">
         <f>IF(E15="",ROUND(1*G15,2),ROUND(E15*G15,2))</f>
         <v>200</v>
       </c>
-      <c r="I15" s="59"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
@@ -2081,11 +2013,11 @@
       <c r="G16" s="40">
         <v>75</v>
       </c>
-      <c r="H16" s="60">
+      <c r="H16" s="59">
         <f>IF(E16="",ROUND(1*G16,2),ROUND(E16*G16,2))</f>
         <v>375</v>
       </c>
-      <c r="I16" s="61"/>
+      <c r="I16" s="60"/>
       <c r="J16" s="13"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2096,8 +2028,8 @@
       <c r="E17" s="30"/>
       <c r="F17" s="36"/>
       <c r="G17" s="40"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="61"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2148,7 +2080,7 @@
       <c r="I21" s="43"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2172,7 +2104,7 @@
       <c r="I23" s="43"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2184,7 +2116,7 @@
       <c r="I24" s="43"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2196,7 +2128,7 @@
       <c r="I25" s="43"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -2208,7 +2140,7 @@
       <c r="I26" s="43"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -2220,7 +2152,7 @@
       <c r="I27" s="43"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -2228,11 +2160,11 @@
       <c r="E28" s="31"/>
       <c r="F28" s="34"/>
       <c r="G28" s="40"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="61"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="60"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2240,11 +2172,11 @@
       <c r="E29" s="31"/>
       <c r="F29" s="34"/>
       <c r="G29" s="40"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="61"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -2252,14 +2184,14 @@
       <c r="E30" s="32"/>
       <c r="F30" s="35"/>
       <c r="G30" s="41"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="63"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="62"/>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="str">
         <f>"("&amp;BAHTTEXT(H38)&amp;")"</f>
         <v>(ห้าร้อยสามสิบห้าบาทยี่สิบเจ็ดสตางค์)</v>
@@ -2268,34 +2200,34 @@
       <c r="G32" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="64">
+      <c r="H32" s="63">
         <f>SUM(H15:H30)</f>
         <v>575</v>
       </c>
-      <c r="I32" s="64"/>
+      <c r="I32" s="63"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="F33" s="24"/>
       <c r="G33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="64">
+      <c r="H33" s="63">
         <f>SUM(F15:F30)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="64"/>
+      <c r="I33" s="63"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="G34" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="64">
+      <c r="H34" s="63">
         <f>H32-H33</f>
         <v>575</v>
       </c>
-      <c r="I34" s="64"/>
+      <c r="I34" s="63"/>
       <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:13" s="4" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2306,11 +2238,11 @@
       <c r="G35" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="64">
+      <c r="H35" s="63">
         <f>H34*0.07</f>
         <v>40.250000000000007</v>
       </c>
-      <c r="I35" s="64"/>
+      <c r="I35" s="63"/>
       <c r="J35" s="6"/>
       <c r="M35"/>
     </row>
@@ -2318,24 +2250,24 @@
       <c r="G36" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="65">
+      <c r="H36" s="64">
         <f>H34+H35</f>
         <v>615.25</v>
       </c>
-      <c r="I36" s="65"/>
+      <c r="I36" s="64"/>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G37" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="64">
+      <c r="H37" s="63">
         <f>H36*0.13</f>
         <v>79.982500000000002</v>
       </c>
-      <c r="I37" s="64"/>
-    </row>
-    <row r="38" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="I37" s="63"/>
+    </row>
+    <row r="38" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -2345,73 +2277,73 @@
       <c r="G38" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="H38" s="66">
+      <c r="H38" s="65">
         <f>H36-H37</f>
         <v>535.26750000000004</v>
       </c>
-      <c r="I38" s="66"/>
+      <c r="I38" s="65"/>
     </row>
     <row r="39" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="67"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="67"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="67"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="66"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+    </row>
+    <row r="42" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A42" s="15"/>
     </row>
-    <row r="43" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="45"/>
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="54"/>
+      <c r="C43" s="67"/>
       <c r="D43" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E43" s="54" t="s">
+      <c r="E43" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54" t="s">
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="I43" s="54"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I43" s="67"/>
+    </row>
+    <row r="44" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A44" s="47"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -2421,24 +2353,21 @@
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="55" t="s">
+    <row r="46" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
       <c r="J46" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="A39:I41"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="H43:I43"/>
     <mergeCell ref="B43:C43"/>
@@ -2455,6 +2384,9 @@
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="A39:I41"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>